<commit_message>
Fixed original data marking, removed kmeans data markings
</commit_message>
<xml_diff>
--- a/Lab4/water-treatmennt-original-marked.xlsx
+++ b/Lab4/water-treatmennt-original-marked.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Alexey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gridb\Machine_learning_2020\nsu_machine_learning_2020\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1931,11 +1931,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN528"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A446" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AN529" sqref="AN529"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" style="1" customWidth="1"/>
+    <col min="8" max="19" width="0" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -10720,7 +10723,7 @@
         <v>99.3</v>
       </c>
       <c r="AN72" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:40" x14ac:dyDescent="0.25">
@@ -12062,7 +12065,7 @@
         <v>99.2</v>
       </c>
       <c r="AN83" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:40" x14ac:dyDescent="0.25">
@@ -12184,7 +12187,7 @@
         <v>99.6</v>
       </c>
       <c r="AN84" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:40" x14ac:dyDescent="0.25">
@@ -12306,7 +12309,7 @@
         <v>99.7</v>
       </c>
       <c r="AN85" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:40" x14ac:dyDescent="0.25">
@@ -12428,7 +12431,7 @@
         <v>100</v>
       </c>
       <c r="AN86" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:40" x14ac:dyDescent="0.25">
@@ -12550,7 +12553,7 @@
         <v>100</v>
       </c>
       <c r="AN87" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:40" x14ac:dyDescent="0.25">
@@ -12672,7 +12675,7 @@
         <v>99.3</v>
       </c>
       <c r="AN88" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:40" x14ac:dyDescent="0.25">
@@ -12794,7 +12797,7 @@
         <v>100</v>
       </c>
       <c r="AN89" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:40" x14ac:dyDescent="0.25">
@@ -12916,7 +12919,7 @@
         <v>99.6</v>
       </c>
       <c r="AN90" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:40" x14ac:dyDescent="0.25">
@@ -13038,7 +13041,7 @@
         <v>99.6</v>
       </c>
       <c r="AN91" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:40" x14ac:dyDescent="0.25">
@@ -13160,7 +13163,7 @@
         <v>99</v>
       </c>
       <c r="AN92" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:40" x14ac:dyDescent="0.25">
@@ -13282,7 +13285,7 @@
         <v>99.7</v>
       </c>
       <c r="AN93" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:40" x14ac:dyDescent="0.25">
@@ -13404,7 +13407,7 @@
         <v>100</v>
       </c>
       <c r="AN94" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:40" x14ac:dyDescent="0.25">
@@ -13770,7 +13773,7 @@
         <v>100</v>
       </c>
       <c r="AN97" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:40" x14ac:dyDescent="0.25">
@@ -13892,7 +13895,7 @@
         <v>100</v>
       </c>
       <c r="AN98" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:40" x14ac:dyDescent="0.25">
@@ -14868,7 +14871,7 @@
         <v>99</v>
       </c>
       <c r="AN106" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:40" x14ac:dyDescent="0.25">
@@ -16332,7 +16335,7 @@
         <v>100</v>
       </c>
       <c r="AN118" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:40" x14ac:dyDescent="0.25">
@@ -16454,7 +16457,7 @@
         <v>100</v>
       </c>
       <c r="AN119" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:40" x14ac:dyDescent="0.25">
@@ -16576,7 +16579,7 @@
         <v>100</v>
       </c>
       <c r="AN120" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:40" x14ac:dyDescent="0.25">
@@ -16942,7 +16945,7 @@
         <v>100</v>
       </c>
       <c r="AN123" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:40" x14ac:dyDescent="0.25">
@@ -17064,7 +17067,7 @@
         <v>100</v>
       </c>
       <c r="AN124" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:40" x14ac:dyDescent="0.25">
@@ -17308,7 +17311,7 @@
         <v>100</v>
       </c>
       <c r="AN126" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:40" x14ac:dyDescent="0.25">
@@ -17552,7 +17555,7 @@
         <v>99.5</v>
       </c>
       <c r="AN128" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:40" x14ac:dyDescent="0.25">
@@ -17674,7 +17677,7 @@
         <v>99.7</v>
       </c>
       <c r="AN129" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:40" x14ac:dyDescent="0.25">
@@ -18284,7 +18287,7 @@
         <v>99.6</v>
       </c>
       <c r="AN134" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:40" x14ac:dyDescent="0.25">
@@ -19382,7 +19385,7 @@
         <v>100</v>
       </c>
       <c r="AN143" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:40" x14ac:dyDescent="0.25">
@@ -19504,7 +19507,7 @@
         <v>96.2</v>
       </c>
       <c r="AN144" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:40" x14ac:dyDescent="0.25">
@@ -19626,7 +19629,7 @@
         <v>99.5</v>
       </c>
       <c r="AN145" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:40" x14ac:dyDescent="0.25">
@@ -19748,7 +19751,7 @@
         <v>98.5</v>
       </c>
       <c r="AN146" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:40" x14ac:dyDescent="0.25">
@@ -19870,7 +19873,7 @@
         <v>92.3</v>
       </c>
       <c r="AN147" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:40" x14ac:dyDescent="0.25">
@@ -20236,7 +20239,7 @@
         <v>100</v>
       </c>
       <c r="AN150" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:40" x14ac:dyDescent="0.25">
@@ -20480,7 +20483,7 @@
         <v>100</v>
       </c>
       <c r="AN152" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:40" x14ac:dyDescent="0.25">
@@ -21090,7 +21093,7 @@
         <v>100</v>
       </c>
       <c r="AN157" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:40" x14ac:dyDescent="0.25">
@@ -21212,7 +21215,7 @@
         <v>100</v>
       </c>
       <c r="AN158" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:40" x14ac:dyDescent="0.25">
@@ -21334,7 +21337,7 @@
         <v>100</v>
       </c>
       <c r="AN159" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:40" x14ac:dyDescent="0.25">
@@ -21822,7 +21825,7 @@
         <v>100</v>
       </c>
       <c r="AN163" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:40" x14ac:dyDescent="0.25">
@@ -21944,7 +21947,7 @@
         <v>100</v>
       </c>
       <c r="AN164" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:40" x14ac:dyDescent="0.25">
@@ -22066,7 +22069,7 @@
         <v>100</v>
       </c>
       <c r="AN165" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:40" x14ac:dyDescent="0.25">
@@ -22310,7 +22313,7 @@
         <v>100</v>
       </c>
       <c r="AN167" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:40" x14ac:dyDescent="0.25">
@@ -22432,7 +22435,7 @@
         <v>98.9</v>
       </c>
       <c r="AN168" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:40" x14ac:dyDescent="0.25">
@@ -22676,7 +22679,7 @@
         <v>98.8</v>
       </c>
       <c r="AN170" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:40" x14ac:dyDescent="0.25">
@@ -22798,7 +22801,7 @@
         <v>100</v>
       </c>
       <c r="AN171" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:40" x14ac:dyDescent="0.25">
@@ -23042,7 +23045,7 @@
         <v>97.8</v>
       </c>
       <c r="AN173" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:40" x14ac:dyDescent="0.25">
@@ -23164,7 +23167,7 @@
         <v>99.5</v>
       </c>
       <c r="AN174" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175" spans="1:40" x14ac:dyDescent="0.25">
@@ -23286,7 +23289,7 @@
         <v>100</v>
       </c>
       <c r="AN175" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:40" x14ac:dyDescent="0.25">
@@ -23408,7 +23411,7 @@
         <v>100</v>
       </c>
       <c r="AN176" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177" spans="1:40" x14ac:dyDescent="0.25">
@@ -23530,7 +23533,7 @@
         <v>99.5</v>
       </c>
       <c r="AN177" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:40" x14ac:dyDescent="0.25">
@@ -23652,7 +23655,7 @@
         <v>99.7</v>
       </c>
       <c r="AN178" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:40" x14ac:dyDescent="0.25">
@@ -24018,7 +24021,7 @@
         <v>100</v>
       </c>
       <c r="AN181" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:40" x14ac:dyDescent="0.25">
@@ -24140,7 +24143,7 @@
         <v>99.5</v>
       </c>
       <c r="AN182" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:40" x14ac:dyDescent="0.25">
@@ -24262,7 +24265,7 @@
         <v>99.3</v>
       </c>
       <c r="AN183" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:40" x14ac:dyDescent="0.25">
@@ -24384,7 +24387,7 @@
         <v>100</v>
       </c>
       <c r="AN184" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" spans="1:40" x14ac:dyDescent="0.25">
@@ -24506,7 +24509,7 @@
         <v>99.6</v>
       </c>
       <c r="AN185" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:40" x14ac:dyDescent="0.25">
@@ -24628,7 +24631,7 @@
         <v>100</v>
       </c>
       <c r="AN186" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:40" x14ac:dyDescent="0.25">
@@ -24872,7 +24875,7 @@
         <v>100</v>
       </c>
       <c r="AN188" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:40" x14ac:dyDescent="0.25">
@@ -24994,7 +24997,7 @@
         <v>100</v>
       </c>
       <c r="AN189" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190" spans="1:40" x14ac:dyDescent="0.25">
@@ -25116,7 +25119,7 @@
         <v>99.2</v>
       </c>
       <c r="AN190" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="191" spans="1:40" x14ac:dyDescent="0.25">
@@ -25238,7 +25241,7 @@
         <v>99.6</v>
       </c>
       <c r="AN191" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:40" x14ac:dyDescent="0.25">
@@ -25360,7 +25363,7 @@
         <v>99.5</v>
       </c>
       <c r="AN192" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="193" spans="1:40" x14ac:dyDescent="0.25">
@@ -25482,7 +25485,7 @@
         <v>100</v>
       </c>
       <c r="AN193" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:40" x14ac:dyDescent="0.25">
@@ -25726,7 +25729,7 @@
         <v>99.7</v>
       </c>
       <c r="AN195" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:40" x14ac:dyDescent="0.25">
@@ -25848,7 +25851,7 @@
         <v>100</v>
       </c>
       <c r="AN196" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:40" x14ac:dyDescent="0.25">
@@ -25970,7 +25973,7 @@
         <v>100</v>
       </c>
       <c r="AN197" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:40" x14ac:dyDescent="0.25">
@@ -26092,7 +26095,7 @@
         <v>100</v>
       </c>
       <c r="AN198" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:40" x14ac:dyDescent="0.25">
@@ -26458,7 +26461,7 @@
         <v>98.6</v>
       </c>
       <c r="AN201" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:40" x14ac:dyDescent="0.25">
@@ -26580,7 +26583,7 @@
         <v>100</v>
       </c>
       <c r="AN202" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:40" x14ac:dyDescent="0.25">
@@ -26702,7 +26705,7 @@
         <v>99.1</v>
       </c>
       <c r="AN203" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:40" x14ac:dyDescent="0.25">
@@ -26824,7 +26827,7 @@
         <v>100</v>
       </c>
       <c r="AN204" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:40" x14ac:dyDescent="0.25">
@@ -26946,7 +26949,7 @@
         <v>100</v>
       </c>
       <c r="AN205" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:40" x14ac:dyDescent="0.25">
@@ -27068,7 +27071,7 @@
         <v>100</v>
       </c>
       <c r="AN206" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:40" x14ac:dyDescent="0.25">
@@ -27922,7 +27925,7 @@
         <v>99.2</v>
       </c>
       <c r="AN213" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="214" spans="1:40" x14ac:dyDescent="0.25">
@@ -29142,7 +29145,7 @@
         <v>99.6</v>
       </c>
       <c r="AN223" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224" spans="1:40" x14ac:dyDescent="0.25">
@@ -29508,7 +29511,7 @@
         <v>100</v>
       </c>
       <c r="AN226" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:40" x14ac:dyDescent="0.25">
@@ -30118,7 +30121,7 @@
         <v>1</v>
       </c>
       <c r="AN231" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:40" x14ac:dyDescent="0.25">
@@ -32558,7 +32561,7 @@
         <v>1</v>
       </c>
       <c r="AN251" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="252" spans="1:40" x14ac:dyDescent="0.25">
@@ -32802,7 +32805,7 @@
         <v>99.8</v>
       </c>
       <c r="AN253" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:40" x14ac:dyDescent="0.25">
@@ -33290,7 +33293,7 @@
         <v>100</v>
       </c>
       <c r="AN257" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="258" spans="1:40" x14ac:dyDescent="0.25">
@@ -33534,7 +33537,7 @@
         <v>99.3</v>
       </c>
       <c r="AN259" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260" spans="1:40" x14ac:dyDescent="0.25">
@@ -33656,7 +33659,7 @@
         <v>99.6</v>
       </c>
       <c r="AN260" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="261" spans="1:40" x14ac:dyDescent="0.25">
@@ -35605,7 +35608,7 @@
         <v>99.2</v>
       </c>
       <c r="AN276" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="277" spans="1:40" x14ac:dyDescent="0.25">
@@ -35727,7 +35730,7 @@
         <v>100</v>
       </c>
       <c r="AN277" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="278" spans="1:40" x14ac:dyDescent="0.25">
@@ -35849,7 +35852,7 @@
         <v>99.8</v>
       </c>
       <c r="AN278" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="279" spans="1:40" x14ac:dyDescent="0.25">
@@ -35971,7 +35974,7 @@
         <v>99.6</v>
       </c>
       <c r="AN279" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="280" spans="1:40" x14ac:dyDescent="0.25">
@@ -36093,7 +36096,7 @@
         <v>99.6</v>
       </c>
       <c r="AN280" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281" spans="1:40" x14ac:dyDescent="0.25">
@@ -37923,7 +37926,7 @@
         <v>99.4</v>
       </c>
       <c r="AN295" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="296" spans="1:40" x14ac:dyDescent="0.25">
@@ -38045,7 +38048,7 @@
         <v>99.4</v>
       </c>
       <c r="AN296" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="297" spans="1:40" x14ac:dyDescent="0.25">
@@ -38655,7 +38658,7 @@
         <v>98.6</v>
       </c>
       <c r="AN301" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:40" x14ac:dyDescent="0.25">
@@ -39387,7 +39390,7 @@
         <v>1</v>
       </c>
       <c r="AN307" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="308" spans="1:40" x14ac:dyDescent="0.25">
@@ -40241,7 +40244,7 @@
         <v>100</v>
       </c>
       <c r="AN314" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="315" spans="1:40" x14ac:dyDescent="0.25">
@@ -41217,7 +41220,7 @@
         <v>100</v>
       </c>
       <c r="AN322" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="323" spans="1:40" x14ac:dyDescent="0.25">
@@ -41583,7 +41586,7 @@
         <v>1</v>
       </c>
       <c r="AN325" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="326" spans="1:40" x14ac:dyDescent="0.25">
@@ -45365,7 +45368,7 @@
         <v>99.9</v>
       </c>
       <c r="AN356" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="357" spans="1:40" x14ac:dyDescent="0.25">
@@ -48781,7 +48784,7 @@
         <v>1</v>
       </c>
       <c r="AN384" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="385" spans="1:40" x14ac:dyDescent="0.25">
@@ -49391,7 +49394,7 @@
         <v>99.8</v>
       </c>
       <c r="AN389" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="390" spans="1:40" x14ac:dyDescent="0.25">
@@ -49757,7 +49760,7 @@
         <v>99.8</v>
       </c>
       <c r="AN392" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="393" spans="1:40" x14ac:dyDescent="0.25">
@@ -50733,7 +50736,7 @@
         <v>99.8</v>
       </c>
       <c r="AN400" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="401" spans="1:40" x14ac:dyDescent="0.25">
@@ -50855,7 +50858,7 @@
         <v>99.6</v>
       </c>
       <c r="AN401" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="402" spans="1:40" x14ac:dyDescent="0.25">
@@ -52441,7 +52444,7 @@
         <v>100</v>
       </c>
       <c r="AN414" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="415" spans="1:40" x14ac:dyDescent="0.25">
@@ -53295,7 +53298,7 @@
         <v>99.7</v>
       </c>
       <c r="AN421" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="422" spans="1:40" x14ac:dyDescent="0.25">
@@ -53539,7 +53542,7 @@
         <v>100</v>
       </c>
       <c r="AN423" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="424" spans="1:40" x14ac:dyDescent="0.25">
@@ -53661,7 +53664,7 @@
         <v>99.7</v>
       </c>
       <c r="AN424" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="425" spans="1:40" x14ac:dyDescent="0.25">
@@ -54637,7 +54640,7 @@
         <v>1</v>
       </c>
       <c r="AN432" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="433" spans="1:40" x14ac:dyDescent="0.25">
@@ -54881,7 +54884,7 @@
         <v>1</v>
       </c>
       <c r="AN434" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="435" spans="1:40" x14ac:dyDescent="0.25">
@@ -55003,7 +55006,7 @@
         <v>99.8</v>
       </c>
       <c r="AN435" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="436" spans="1:40" x14ac:dyDescent="0.25">
@@ -56223,7 +56226,7 @@
         <v>100</v>
       </c>
       <c r="AN445" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="446" spans="1:40" x14ac:dyDescent="0.25">
@@ -56833,7 +56836,7 @@
         <v>99.3</v>
       </c>
       <c r="AN450" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="451" spans="1:40" x14ac:dyDescent="0.25">
@@ -57809,7 +57812,7 @@
         <v>99.8</v>
       </c>
       <c r="AN458" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="459" spans="1:40" x14ac:dyDescent="0.25">
@@ -58297,7 +58300,7 @@
         <v>99.7</v>
       </c>
       <c r="AN462" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="463" spans="1:40" x14ac:dyDescent="0.25">
@@ -58419,7 +58422,7 @@
         <v>100</v>
       </c>
       <c r="AN463" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="464" spans="1:40" x14ac:dyDescent="0.25">
@@ -58663,7 +58666,7 @@
         <v>1</v>
       </c>
       <c r="AN465" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="466" spans="1:40" x14ac:dyDescent="0.25">
@@ -60371,7 +60374,7 @@
         <v>99.7</v>
       </c>
       <c r="AN479" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="480" spans="1:40" x14ac:dyDescent="0.25">
@@ -60981,7 +60984,7 @@
         <v>99.2</v>
       </c>
       <c r="AN484" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="485" spans="1:40" x14ac:dyDescent="0.25">
@@ -61103,7 +61106,7 @@
         <v>99.6</v>
       </c>
       <c r="AN485" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="486" spans="1:40" x14ac:dyDescent="0.25">
@@ -61225,7 +61228,7 @@
         <v>99.7</v>
       </c>
       <c r="AN486" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="487" spans="1:40" x14ac:dyDescent="0.25">
@@ -61469,7 +61472,7 @@
         <v>98.2</v>
       </c>
       <c r="AN488" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="489" spans="1:40" x14ac:dyDescent="0.25">
@@ -61713,7 +61716,7 @@
         <v>99.7</v>
       </c>
       <c r="AN490" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="491" spans="1:40" x14ac:dyDescent="0.25">
@@ -66232,8 +66235,8 @@
     </row>
     <row r="528" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AN528" s="1">
-        <f xml:space="preserve"> COUNTIF(AN1:AN527, 1)</f>
-        <v>394</v>
+        <f xml:space="preserve"> COUNTIF(AN1:AN527, 5)</f>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>